<commit_message>
Added a 1475.HK Model
</commit_message>
<xml_diff>
--- a/financial_models/opportunities/1910.HK_Stock_Valuation.xlsx
+++ b/financial_models/opportunities/1910.HK_Stock_Valuation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b10873df2abd437/文档/Company_Investment/Opportunities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{81CC1E11-8769-7346-B8E7-77899CF1825C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA17CFBE-0FB0-2F40-BAB2-AABC2674FE78}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="8_{81CC1E11-8769-7346-B8E7-77899CF1825C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CDBF5E5-EE21-0D4F-A6AA-D240A828DEEB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,15 +45,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="230">
   <si>
     <t>Company Info:</t>
-  </si>
-  <si>
-    <t>Ticker:</t>
-  </si>
-  <si>
-    <t>Ticker Name:</t>
   </si>
   <si>
     <t>Current Price:</t>
@@ -726,9 +720,6 @@
     <t>Normalized E/P</t>
   </si>
   <si>
-    <t>Normalized D/P:</t>
-  </si>
-  <si>
     <t>US Riskfree</t>
   </si>
   <si>
@@ -798,13 +789,25 @@
     <t>US</t>
   </si>
   <si>
-    <t>Watchlist:</t>
-  </si>
-  <si>
     <t>Market Yields</t>
   </si>
   <si>
     <t>Non-controlling Interests</t>
+  </si>
+  <si>
+    <t>Watchlist &amp; Comp_Group:</t>
+  </si>
+  <si>
+    <t>C0001</t>
+  </si>
+  <si>
+    <t>Normalized D/P</t>
+  </si>
+  <si>
+    <t>Symbol:</t>
+  </si>
+  <si>
+    <t>Name:</t>
   </si>
 </sst>
 </file>
@@ -1279,7 +1282,7 @@
     <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1706,14 +1709,45 @@
     <xf numFmtId="10" fontId="2" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="13" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1728,36 +1762,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="2" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2096,7 +2102,7 @@
   <dimension ref="A1:J923"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2137,69 +2143,69 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="191" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" s="192"/>
+        <v>228</v>
+      </c>
+      <c r="C3" s="198" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="199"/>
       <c r="E3" s="94"/>
       <c r="F3" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3" s="171">
         <v>19.04</v>
       </c>
       <c r="H3" s="173" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="203" t="s">
-        <v>222</v>
-      </c>
-      <c r="D4" s="204"/>
+        <v>229</v>
+      </c>
+      <c r="C4" s="200" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="201"/>
       <c r="E4" s="94"/>
       <c r="F4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="200">
+        <v>3</v>
+      </c>
+      <c r="G4" s="204">
         <v>1462217799</v>
       </c>
-      <c r="H4" s="200"/>
+      <c r="H4" s="204"/>
       <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C5" s="202">
         <v>45591</v>
       </c>
-      <c r="D5" s="193"/>
+      <c r="D5" s="203"/>
       <c r="E5" s="34"/>
       <c r="F5" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="G5" s="190">
+        <v>103</v>
+      </c>
+      <c r="G5" s="196">
         <f>G3*G4/1000000</f>
         <v>27840.626892959997</v>
       </c>
-      <c r="H5" s="190"/>
+      <c r="H5" s="196"/>
       <c r="I5" s="38"/>
       <c r="J5" s="28"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="94" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="205">
+        <v>4</v>
+      </c>
+      <c r="C6" s="191">
         <v>8</v>
       </c>
-      <c r="D6" s="206">
+      <c r="D6" s="192">
         <f>EOMONTH(EDATE(Fin_Analysis!D9,C6),0)</f>
         <v>45716</v>
       </c>
@@ -2208,25 +2214,27 @@
         <v>45291</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="207" t="s">
-        <v>224</v>
-      </c>
-      <c r="H6" s="207"/>
+        <v>5</v>
+      </c>
+      <c r="G6" s="197" t="s">
+        <v>221</v>
+      </c>
+      <c r="H6" s="197"/>
       <c r="I6" s="38"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="C7" s="190" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="212" t="s">
         <v>226</v>
       </c>
-      <c r="C7" s="203" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="204"/>
       <c r="E7" s="94"/>
       <c r="F7" s="35" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G7" s="172">
         <v>7.8</v>
@@ -2239,45 +2247,45 @@
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="180" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F9" s="186" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C10" s="170">
         <v>4.0899999999999999E-2</v>
       </c>
       <c r="F10" s="125" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="147" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C11" s="184">
         <v>5.1499999999999997E-2</v>
       </c>
       <c r="D11" s="177" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F11" s="125" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B12" s="94" t="s">
-        <v>145</v>
-      </c>
-      <c r="C12" s="208">
+        <v>143</v>
+      </c>
+      <c r="C12" s="193">
         <v>0.08</v>
       </c>
-      <c r="D12" s="209">
+      <c r="D12" s="170">
         <f>(C12+C17)/2</f>
         <v>9.6250000000000002E-2</v>
       </c>
@@ -2286,45 +2294,45 @@
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C14" s="170">
         <v>2.0799999999999999E-2</v>
       </c>
       <c r="F14" s="125" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C15" s="170">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F15" s="125" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="147" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C16" s="184">
         <v>0.16</v>
       </c>
-      <c r="D16" s="211" t="s">
-        <v>221</v>
+      <c r="D16" s="195" t="s">
+        <v>218</v>
       </c>
       <c r="F16" s="125" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B17" s="94" t="s">
-        <v>209</v>
-      </c>
-      <c r="C17" s="210">
+        <v>206</v>
+      </c>
+      <c r="C17" s="194">
         <f>(C15+C16)/2</f>
         <v>0.1125</v>
       </c>
@@ -2333,29 +2341,29 @@
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="185" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C19" s="175" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D19" s="94"/>
       <c r="E19" s="94"/>
       <c r="F19" s="185" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G19" s="94"/>
       <c r="H19" s="94"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="177" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C20" s="178">
         <f>Fin_Analysis!F75</f>
         <v>0.40723441233977836</v>
       </c>
       <c r="F20" s="181" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G20" s="178">
         <f>Fin_Analysis!F91</f>
@@ -2364,14 +2372,14 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="177" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C21" s="178">
         <f>Fin_Analysis!F77</f>
         <v>0.41258418422767756</v>
       </c>
       <c r="F21" s="181" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G21" s="178">
         <f>Fin_Analysis!F92</f>
@@ -2380,26 +2388,26 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="177" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C22" s="178">
         <f>Fin_Analysis!F79</f>
         <v>4.6980230284597004E-2</v>
       </c>
       <c r="F22" s="185" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="177" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C23" s="178">
         <f>Fin_Analysis!F80</f>
         <v>0</v>
       </c>
       <c r="F23" s="181" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G23" s="188">
         <f>G3/(Data!C34*Data!E3/Common_Shares*Exchange_Rate)</f>
@@ -2408,14 +2416,14 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="177" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C24" s="178">
         <f>Fin_Analysis!F82</f>
         <v>9.0430154247230065E-3</v>
       </c>
       <c r="F24" s="181" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G24" s="182">
         <f>(Fin_Analysis!E86*G7)/G3</f>
@@ -2424,14 +2432,14 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="177" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C25" s="178">
         <f>Fin_Analysis!F82</f>
         <v>9.0430154247230065E-3</v>
       </c>
       <c r="F25" s="181" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G25" s="178">
         <f>Fin_Analysis!F87</f>
@@ -2440,14 +2448,14 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="179" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C26" s="178">
         <f>Fin_Analysis!F83</f>
         <v>0.12160756362907141</v>
       </c>
       <c r="F26" s="183" t="s">
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="G26" s="182">
         <f>Fin_Analysis!E87*Exchange_Rate/G3</f>
@@ -2458,24 +2466,24 @@
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="5"/>
       <c r="B28" s="99" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C28" s="98" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D28" s="43" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E28" s="62"/>
       <c r="F28" s="53" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G28" s="93"/>
       <c r="H28" s="93"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="94" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C29" s="168">
         <f>IF(Fin_Analysis!C103="Profit",Fin_Analysis!E98,Fin_Analysis!E101)</f>
@@ -3387,14 +3395,13 @@
     <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="C11:C12 C16:C17">
@@ -3421,7 +3428,7 @@
     <dataValidation type="list" allowBlank="1" sqref="G6" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"HKD,USD,CNY,EUR"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D7" xr:uid="{3894A86A-E1B4-A843-BE8E-14D1CE0AE26E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{3894A86A-E1B4-A843-BE8E-14D1CE0AE26E}">
       <formula1>"Y, N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3469,7 +3476,7 @@
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16"/>
       <c r="B2" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="17"/>
@@ -3486,13 +3493,13 @@
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
       <c r="B3" s="116" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="96">
         <v>45291</v>
       </c>
       <c r="D3" s="116" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="92">
         <v>1000000</v>
@@ -3518,7 +3525,7 @@
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="16"/>
       <c r="B5" s="140" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" s="48">
         <f>C3</f>
@@ -3568,7 +3575,7 @@
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" s="105" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="58">
         <v>3682.4</v>
@@ -3590,7 +3597,7 @@
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="107" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="103">
         <f t="shared" ref="C7:M7" si="1">IF(D6="","",C6/D6-1)</f>
@@ -3641,7 +3648,7 @@
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="108" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C8" s="92">
         <v>1499.6</v>
@@ -3663,7 +3670,7 @@
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="109" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C9" s="101">
         <f t="shared" ref="C9:M9" si="2">IF(C6="","",(C6-C8))</f>
@@ -3714,7 +3721,7 @@
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="108" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" s="92">
         <v>1519.3</v>
@@ -3736,7 +3743,7 @@
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="105" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C11" s="97">
         <f t="shared" ref="C11:M11" si="3">IF(C6="","",(C12/C6))</f>
@@ -3787,7 +3794,7 @@
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="108" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C12" s="92"/>
       <c r="D12" s="92"/>
@@ -3805,7 +3812,7 @@
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="109" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C13" s="101">
         <f>IF(C6="","",(C9-C10+C12))</f>
@@ -3856,7 +3863,7 @@
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="108" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" s="92"/>
       <c r="D14" s="92"/>
@@ -3874,7 +3881,7 @@
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="108" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C15" s="92"/>
       <c r="D15" s="92"/>
@@ -3892,7 +3899,7 @@
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="108" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C16" s="92"/>
       <c r="D16" s="92"/>
@@ -3910,7 +3917,7 @@
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="108" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C17" s="92">
         <v>173</v>
@@ -3932,7 +3939,7 @@
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4"/>
       <c r="B18" s="110" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C18" s="92">
         <v>33.299999999999997</v>
@@ -3954,7 +3961,7 @@
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="105" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C19" s="95">
         <f>IF(C6="","",C13-C14-MAX(C15,0)-MAX(C16,0)-C17-MAX(C18/(1-Fin_Analysis!$F$84),0))</f>
@@ -4005,7 +4012,7 @@
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
       <c r="B20" s="109" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C20" s="57">
         <f>IF(D19="","",IF(ABS(C19+D19)=ABS(C19)+ABS(D19),IF(C19&lt;0,-1,1)*(C19-D19)/D19,"Turn"))</f>
@@ -4056,7 +4063,7 @@
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21" s="111" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C21" s="56">
         <f t="shared" ref="C21:M21" si="6">IF(C6="","",C22/C6)</f>
@@ -4107,7 +4114,7 @@
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4"/>
       <c r="B22" s="113" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C22" s="102">
         <f>IF(C6="","",C19*(1-Fin_Analysis!$F$84))</f>
@@ -4158,7 +4165,7 @@
     <row r="23" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="112" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C23" s="80">
         <f>IF(D22="","",IF(ABS(C22+D22)=ABS(C22)+ABS(D22),IF(C22&lt;0,-1,1)*(C22-D22)/D22,"Turn"))</f>
@@ -4209,7 +4216,7 @@
     <row r="24" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A24" s="16"/>
       <c r="B24" s="139" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C24" s="48">
         <f>Fin_Analysis!D9</f>
@@ -4260,7 +4267,7 @@
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4"/>
       <c r="B25" s="105" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C25" s="41">
         <f t="shared" ref="C25:M25" si="17">IF(C6="","",C34+C29+C30)</f>
@@ -4311,7 +4318,7 @@
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4"/>
       <c r="B26" s="105" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C26" s="41">
         <f>Fin_Analysis!C28</f>
@@ -4332,7 +4339,7 @@
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4"/>
       <c r="B27" s="105" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C27" s="41">
         <f>Fin_Analysis!C13</f>
@@ -4353,7 +4360,7 @@
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4"/>
       <c r="B28" s="105" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C28" s="41">
         <f>Fin_Analysis!C18</f>
@@ -4374,7 +4381,7 @@
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4"/>
       <c r="B29" s="105" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C29" s="41">
         <f>Fin_Analysis!I28</f>
@@ -4395,7 +4402,7 @@
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4"/>
       <c r="B30" s="105" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C30" s="41">
         <f>Fin_Analysis!I48</f>
@@ -4416,7 +4423,7 @@
     <row r="31" spans="1:14" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4"/>
       <c r="B31" s="105" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C31" s="41">
         <f>Fin_Analysis!I15</f>
@@ -4437,7 +4444,7 @@
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4"/>
       <c r="B32" s="105" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C32" s="41">
         <f>Fin_Analysis!I34</f>
@@ -4458,7 +4465,7 @@
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4"/>
       <c r="B33" s="105" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C33" s="95">
         <f t="shared" ref="C33:M33" si="18">IF(C6="","",C31+C32)</f>
@@ -4509,7 +4516,7 @@
     <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4"/>
       <c r="B34" s="105" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C34" s="41">
         <f>Fin_Analysis!D3</f>
@@ -4530,7 +4537,7 @@
     <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="4"/>
       <c r="B35" s="105" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C35" s="41">
         <f>Fin_Analysis!D4</f>
@@ -4551,7 +4558,7 @@
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="4"/>
       <c r="B36" s="105" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C36" s="41">
         <f>Fin_Analysis!C63</f>
@@ -4572,7 +4579,7 @@
     <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="4"/>
       <c r="B37" s="105" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C37" s="41">
         <f>Fin_Analysis!C68</f>
@@ -4623,7 +4630,7 @@
     <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4"/>
       <c r="B38" s="109" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C38" s="104">
         <f>IF(C6="","",C19/C37)</f>
@@ -4674,7 +4681,7 @@
     <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="16"/>
       <c r="B39" s="55" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C39" s="54"/>
       <c r="D39" s="54"/>
@@ -4692,7 +4699,7 @@
     <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4"/>
       <c r="B40" s="106" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C40" s="61">
         <f t="shared" ref="C40:M40" si="21">IF(C6="","",C8/C6)</f>
@@ -4743,7 +4750,7 @@
     <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4"/>
       <c r="B41" s="105" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C41" s="56">
         <f t="shared" ref="C41:M41" si="22">IF(C6="","",(C10-C12)/C6)</f>
@@ -4794,7 +4801,7 @@
     <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="4"/>
       <c r="B42" s="105" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C42" s="56">
         <f t="shared" ref="C42:M42" si="23">IF(C6="","",(C14+MAX(C15,0))/C6)</f>
@@ -4845,7 +4852,7 @@
     <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="4"/>
       <c r="B43" s="105" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C43" s="56">
         <f t="shared" ref="C43:M43" si="24">IF(C6="","",MAX(C16,0)/C6)</f>
@@ -4896,7 +4903,7 @@
     <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="4"/>
       <c r="B44" s="105" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C44" s="56">
         <f t="shared" ref="C44:M44" si="25">IF(C6="","",C17/C6)</f>
@@ -4947,7 +4954,7 @@
     <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="4"/>
       <c r="B45" s="105" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C45" s="56">
         <f>IF(C6="","",MAX(C18,0)/(1-Fin_Analysis!$F$84)/C6)</f>
@@ -4998,7 +5005,7 @@
     <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="4"/>
       <c r="B46" s="105" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C46" s="56">
         <f t="shared" ref="C46:M46" si="26">IF(C6="","",C19/C6)</f>
@@ -5049,7 +5056,7 @@
     <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="16"/>
       <c r="B47" s="114" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C47" s="36"/>
       <c r="D47" s="36"/>
@@ -5067,7 +5074,7 @@
     <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4"/>
       <c r="B48" s="106" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C48" s="61">
         <f t="shared" ref="C48:M48" si="27">IF(C6="","",C27/C6)</f>
@@ -5118,7 +5125,7 @@
     <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4"/>
       <c r="B49" s="105" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C49" s="56">
         <f t="shared" ref="C49:M49" si="28">IF(C6="","",C28/C6)</f>
@@ -5169,7 +5176,7 @@
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="16"/>
       <c r="B50" s="114" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C50" s="36"/>
       <c r="D50" s="36"/>
@@ -5186,7 +5193,7 @@
     <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="4"/>
       <c r="B51" s="106" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C51" s="61">
         <f>IF(C34="","",(C25-C34)/C25)</f>
@@ -5236,7 +5243,7 @@
     <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="4"/>
       <c r="B52" s="105" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C52" s="60">
         <f t="shared" ref="C52:M52" si="30">IF(C19="","",IF(C33&lt;=0,"-",C19/C33))</f>
@@ -5286,7 +5293,7 @@
     <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="4"/>
       <c r="B53" s="105" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C53" s="56">
         <f t="shared" ref="C53:M53" si="31">IF(C19="","",IF(C17&lt;=0,"-",C17/C19))</f>
@@ -5336,7 +5343,7 @@
     <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="4"/>
       <c r="B54" s="109" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C54" s="62">
         <f t="shared" ref="C54:M54" si="32">IF(C26="","",C26/C29)</f>
@@ -6691,7 +6698,7 @@
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="45" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="45"/>
       <c r="D2" s="68"/>
@@ -6701,12 +6708,12 @@
       <c r="H2" s="7"/>
       <c r="I2" s="94"/>
       <c r="K2" s="50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="94"/>
       <c r="D3" s="141">
@@ -6720,7 +6727,7 @@
       <c r="F3" s="94"/>
       <c r="G3" s="94"/>
       <c r="H3" s="47" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I3" s="59">
         <v>1478.9</v>
@@ -6729,7 +6736,7 @@
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="94"/>
       <c r="D4" s="69">
@@ -6747,10 +6754,10 @@
       <c r="C5" s="94"/>
       <c r="D5" s="94"/>
       <c r="E5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="I5" s="67">
         <f>C28/I28</f>
@@ -6760,7 +6767,7 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="94"/>
       <c r="D6" s="75">
@@ -6774,7 +6781,7 @@
       <c r="F6" s="94"/>
       <c r="G6" s="94"/>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I6" s="67">
         <f>(C24+C25)/I28</f>
@@ -6785,7 +6792,7 @@
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B7" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="94"/>
       <c r="D7" s="70">
@@ -6797,7 +6804,7 @@
         <v>HKD</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I7" s="67">
         <f>C24/I28</f>
@@ -6815,7 +6822,7 @@
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="93"/>
       <c r="D9" s="71">
@@ -6833,32 +6840,32 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="81" t="s">
+      <c r="E10" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="81" t="s">
+      <c r="F10" s="126" t="s">
         <v>37</v>
-      </c>
-      <c r="E10" s="81" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="126" t="s">
-        <v>39</v>
       </c>
       <c r="G10" s="94"/>
       <c r="H10" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I10" s="81" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K10" s="24"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="63">
         <v>815.5</v>
@@ -6873,7 +6880,7 @@
       <c r="F11" s="127"/>
       <c r="G11" s="94"/>
       <c r="H11" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I11" s="63">
         <f>67.8+25</f>
@@ -6884,7 +6891,7 @@
     </row>
     <row r="12" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C12" s="63"/>
       <c r="D12" s="64">
@@ -6897,7 +6904,7 @@
       <c r="F12" s="127"/>
       <c r="G12" s="94"/>
       <c r="H12" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I12" s="63">
         <v>126</v>
@@ -6907,7 +6914,7 @@
     </row>
     <row r="13" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="B13" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C13" s="63">
         <v>346.1</v>
@@ -6922,7 +6929,7 @@
       <c r="F13" s="127"/>
       <c r="G13" s="94"/>
       <c r="H13" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I13" s="63"/>
       <c r="J13" s="94"/>
@@ -6930,7 +6937,7 @@
     </row>
     <row r="14" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="63"/>
       <c r="D14" s="64">
@@ -6943,7 +6950,7 @@
       <c r="F14" s="127"/>
       <c r="G14" s="94"/>
       <c r="H14" s="93" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I14" s="145"/>
       <c r="J14" s="94"/>
@@ -6951,7 +6958,7 @@
     </row>
     <row r="15" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" s="63"/>
       <c r="D15" s="64">
@@ -6964,7 +6971,7 @@
       <c r="F15" s="127"/>
       <c r="G15" s="94"/>
       <c r="H15" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I15" s="91">
         <f>SUM(I11:I14)</f>
@@ -6974,7 +6981,7 @@
     </row>
     <row r="16" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C16" s="63"/>
       <c r="D16" s="64">
@@ -6992,7 +6999,7 @@
     </row>
     <row r="17" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B17" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C17" s="63">
         <v>95.8</v>
@@ -7012,7 +7019,7 @@
     </row>
     <row r="18" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" s="63">
         <v>637.70000000000005</v>
@@ -7031,7 +7038,7 @@
     </row>
     <row r="19" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" s="63"/>
       <c r="D19" s="64">
@@ -7042,7 +7049,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="128" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G19" s="30">
         <f>IF(F19="Y",0,1)</f>
@@ -7051,7 +7058,7 @@
     </row>
     <row r="20" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B20" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C20" s="63"/>
       <c r="D20" s="64">
@@ -7062,7 +7069,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="128" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G20" s="30">
         <f>IF(F20="Y",0,1)</f>
@@ -7073,7 +7080,7 @@
     </row>
     <row r="21" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B21" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" s="63"/>
       <c r="D21" s="64">
@@ -7090,7 +7097,7 @@
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" s="63"/>
       <c r="D22" s="64">
@@ -7103,7 +7110,7 @@
       <c r="F22" s="127"/>
       <c r="G22" s="94"/>
       <c r="H22" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I22" s="52">
         <f>I28-SUM(I11:I14)</f>
@@ -7115,13 +7122,13 @@
       <c r="D23" s="94"/>
       <c r="E23" s="94"/>
       <c r="F23" s="126" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G23" s="94"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24" s="65">
         <f>SUM(C11:C14)</f>
@@ -7143,7 +7150,7 @@
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C25" s="65">
         <f>SUM(C15:C17)</f>
@@ -7163,7 +7170,7 @@
       </c>
       <c r="G25" s="94"/>
       <c r="H25" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I25" s="67">
         <f>E28/I28</f>
@@ -7172,7 +7179,7 @@
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C26" s="65">
         <f>C18+C19+C20</f>
@@ -7192,7 +7199,7 @@
       </c>
       <c r="G26" s="94"/>
       <c r="H26" s="23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I26" s="67">
         <f>E24/($I$28-I22)</f>
@@ -7205,7 +7212,7 @@
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C27" s="84">
         <f>C21+C22</f>
@@ -7225,7 +7232,7 @@
       </c>
       <c r="G27" s="94"/>
       <c r="H27" s="23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I27" s="67">
         <f>(E25+E24)/$I$28</f>
@@ -7238,7 +7245,7 @@
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="85" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28" s="86">
         <f>SUM(C11:C22)</f>
@@ -7255,7 +7262,7 @@
       <c r="F28" s="127"/>
       <c r="G28" s="94"/>
       <c r="H28" s="85" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I28" s="72">
         <v>1180.4000000000001</v>
@@ -7270,7 +7277,7 @@
       <c r="D29" s="94"/>
       <c r="E29" s="94"/>
       <c r="F29" s="127" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G29" s="94"/>
       <c r="H29" s="94"/>
@@ -7279,7 +7286,7 @@
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C30" s="63"/>
       <c r="D30" s="64">
@@ -7291,7 +7298,7 @@
       <c r="F30" s="127"/>
       <c r="G30" s="94"/>
       <c r="H30" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I30" s="63">
         <v>1721</v>
@@ -7300,7 +7307,7 @@
     </row>
     <row r="31" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C31" s="63"/>
       <c r="D31" s="64">
@@ -7313,7 +7320,7 @@
       <c r="F31" s="127"/>
       <c r="G31" s="94"/>
       <c r="H31" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I31" s="63">
         <v>392.6</v>
@@ -7322,7 +7329,7 @@
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C32" s="63"/>
       <c r="D32" s="64">
@@ -7335,14 +7342,14 @@
       <c r="F32" s="127"/>
       <c r="G32" s="94"/>
       <c r="H32" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I32" s="63"/>
       <c r="J32" s="94"/>
     </row>
     <row r="33" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C33" s="63"/>
       <c r="D33" s="64">
@@ -7358,7 +7365,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="93" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I33" s="145">
         <f>121+0.2</f>
@@ -7368,7 +7375,7 @@
     </row>
     <row r="34" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B34" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C34" s="63"/>
       <c r="D34" s="64">
@@ -7381,7 +7388,7 @@
       <c r="F34" s="127"/>
       <c r="G34" s="94"/>
       <c r="H34" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I34" s="91">
         <f>SUM(I30:I33)</f>
@@ -7391,7 +7398,7 @@
     </row>
     <row r="35" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B35" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C35" s="63"/>
       <c r="D35" s="64">
@@ -7402,7 +7409,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="128" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G35" s="30">
         <f>IF(F35="Y",0,1)</f>
@@ -7412,7 +7419,7 @@
     </row>
     <row r="36" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B36" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C36" s="63"/>
       <c r="D36" s="64">
@@ -7423,7 +7430,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="128" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G36" s="30">
         <f>IF(F36="Y",0,1)</f>
@@ -7434,7 +7441,7 @@
     </row>
     <row r="37" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C37" s="63"/>
       <c r="D37" s="64">
@@ -7445,7 +7452,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="128" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G37" s="30">
         <f>IF(F37="Y",0,1)</f>
@@ -7456,7 +7463,7 @@
     </row>
     <row r="38" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C38" s="63">
         <f>231.7+470.1</f>
@@ -7476,7 +7483,7 @@
     </row>
     <row r="39" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B39" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C39" s="63"/>
       <c r="D39" s="64">
@@ -7493,7 +7500,7 @@
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" s="63">
         <v>1525.3</v>
@@ -7512,7 +7519,7 @@
     </row>
     <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C41" s="63">
         <v>169.3</v>
@@ -7531,7 +7538,7 @@
     </row>
     <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C42" s="63">
         <f>882.1+67.5</f>
@@ -7547,7 +7554,7 @@
       <c r="F42" s="127"/>
       <c r="G42" s="94"/>
       <c r="H42" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I42" s="52">
         <f>I48-SUM(I30:I33)</f>
@@ -7565,7 +7572,7 @@
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C44" s="65">
         <f>SUM(C30:C31)</f>
@@ -7584,7 +7591,7 @@
     </row>
     <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C45" s="65">
         <f>SUM(C32:C35)</f>
@@ -7603,7 +7610,7 @@
     </row>
     <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C46" s="65">
         <f>C36+C37+C38+C39</f>
@@ -7620,7 +7627,7 @@
       <c r="F46" s="94"/>
       <c r="G46" s="94"/>
       <c r="H46" s="23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I46" s="67">
         <f>(E44+E24)/E64</f>
@@ -7633,7 +7640,7 @@
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C47" s="65">
         <f>C40+C41+C42</f>
@@ -7650,7 +7657,7 @@
       <c r="F47" s="94"/>
       <c r="G47" s="94"/>
       <c r="H47" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I47" s="67">
         <f>(E44+E45+E24+E25)/$I$49</f>
@@ -7663,7 +7670,7 @@
     </row>
     <row r="48" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B48" s="87" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C48" s="88">
         <f>SUM(C30:C42)</f>
@@ -7680,7 +7687,7 @@
       <c r="F48" s="94"/>
       <c r="G48" s="94"/>
       <c r="H48" s="87" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I48" s="90">
         <v>2453.6999999999998</v>
@@ -7689,7 +7696,7 @@
     </row>
     <row r="49" spans="2:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B49" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C49" s="65">
         <f>C28+C48</f>
@@ -7706,7 +7713,7 @@
       <c r="F49" s="94"/>
       <c r="G49" s="94"/>
       <c r="H49" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I49" s="52">
         <f>I28+I48</f>
@@ -7722,14 +7729,14 @@
     </row>
     <row r="51" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B51" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C51" s="31"/>
       <c r="D51" s="18"/>
     </row>
     <row r="52" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B52" s="44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C52" s="94"/>
       <c r="D52" s="81" t="str">
@@ -7740,13 +7747,13 @@
       <c r="F52" s="94"/>
       <c r="G52" s="94"/>
       <c r="H52" s="50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I52" s="94"/>
     </row>
     <row r="53" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B53" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C53" s="95">
         <f>D4</f>
@@ -7776,7 +7783,7 @@
     </row>
     <row r="55" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B55" s="25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C55" s="3"/>
       <c r="E55" s="159"/>
@@ -7787,14 +7794,14 @@
     </row>
     <row r="56" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B56" s="20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C56" s="94"/>
-      <c r="D56" s="198">
+      <c r="D56" s="209">
         <f>I15+I34</f>
         <v>2453.6</v>
       </c>
-      <c r="E56" s="199"/>
+      <c r="E56" s="210"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="94"/>
@@ -7802,28 +7809,28 @@
     </row>
     <row r="57" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B57" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C57" s="94"/>
-      <c r="D57" s="200">
+      <c r="D57" s="204">
         <v>0</v>
       </c>
-      <c r="E57" s="193"/>
+      <c r="E57" s="203"/>
       <c r="G57" s="94"/>
       <c r="H57" s="94" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I57" s="94"/>
     </row>
     <row r="58" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C58" s="94"/>
-      <c r="D58" s="200">
+      <c r="D58" s="204">
         <v>0</v>
       </c>
-      <c r="E58" s="193"/>
+      <c r="E58" s="203"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="94"/>
@@ -7840,11 +7847,11 @@
     </row>
     <row r="60" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B60" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="82" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E60" s="94"/>
       <c r="F60" s="9"/>
@@ -7854,7 +7861,7 @@
     </row>
     <row r="61" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B61" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C61" s="74">
         <f>C14+C15+(C19*G19)+(C20*G20)+C31+C32+(C35*G35)+(C36*G36)+(C37*G37)</f>
@@ -7875,7 +7882,7 @@
     </row>
     <row r="62" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B62" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C62" s="142">
         <f>C11+C30</f>
@@ -7896,7 +7903,7 @@
     </row>
     <row r="63" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B63" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C63" s="74">
         <f>C61+C62</f>
@@ -7917,7 +7924,7 @@
     </row>
     <row r="64" spans="2:10" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B64" s="146" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C64" s="147"/>
       <c r="D64" s="148"/>
@@ -7932,7 +7939,7 @@
     </row>
     <row r="65" spans="1:9" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B65" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C65" s="74">
         <f>C63-E64</f>
@@ -7963,11 +7970,11 @@
     </row>
     <row r="67" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B67" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="82" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E67" s="65"/>
       <c r="F67" s="94"/>
@@ -7977,7 +7984,7 @@
     </row>
     <row r="68" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B68" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C68" s="74">
         <f>C49-C63</f>
@@ -7998,7 +8005,7 @@
     </row>
     <row r="69" spans="1:9" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B69" s="146" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C69" s="147"/>
       <c r="D69" s="148"/>
@@ -8013,7 +8020,7 @@
     </row>
     <row r="70" spans="1:9" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B70" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C70" s="74">
         <f>C68-E69</f>
@@ -8035,15 +8042,15 @@
     <row r="72" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="5"/>
       <c r="B72" s="120" t="s">
-        <v>140</v>
-      </c>
-      <c r="C72" s="196">
+        <v>138</v>
+      </c>
+      <c r="C72" s="207">
         <f>Data!C5</f>
         <v>45291</v>
       </c>
-      <c r="D72" s="196"/>
+      <c r="D72" s="207"/>
       <c r="H72" s="50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -8051,18 +8058,18 @@
         <f>"(Numbers in "&amp;Data!E3&amp;Dashboard!G6&amp;")"</f>
         <v>(Numbers in 1000000USD)</v>
       </c>
-      <c r="C73" s="195" t="s">
-        <v>106</v>
-      </c>
-      <c r="D73" s="195"/>
-      <c r="E73" s="197" t="s">
-        <v>107</v>
-      </c>
-      <c r="F73" s="195"/>
+      <c r="C73" s="206" t="s">
+        <v>104</v>
+      </c>
+      <c r="D73" s="206"/>
+      <c r="E73" s="208" t="s">
+        <v>105</v>
+      </c>
+      <c r="F73" s="206"/>
     </row>
     <row r="74" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B74" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C74" s="95">
         <f>Data!C6</f>
@@ -8077,7 +8084,7 @@
     </row>
     <row r="75" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B75" s="117" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C75" s="95">
         <f>Data!C8</f>
@@ -8098,7 +8105,7 @@
     </row>
     <row r="76" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B76" s="35" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C76" s="118">
         <f>C74-C75</f>
@@ -8113,7 +8120,7 @@
     </row>
     <row r="77" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B77" s="117" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C77" s="95">
         <f>Data!C10-Data!C12</f>
@@ -8134,7 +8141,7 @@
     </row>
     <row r="78" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B78" s="35" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C78" s="118">
         <f>C76-C77</f>
@@ -8149,7 +8156,7 @@
     </row>
     <row r="79" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B79" s="117" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C79" s="95">
         <f>Data!C17</f>
@@ -8170,7 +8177,7 @@
     </row>
     <row r="80" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B80" s="28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C80" s="95">
         <f>Data!C14+MAX(Data!C15,0)</f>
@@ -8190,7 +8197,7 @@
     </row>
     <row r="81" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B81" s="28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C81" s="95">
         <f>MAX(Data!C16,0)</f>
@@ -8209,12 +8216,12 @@
         <v>0</v>
       </c>
       <c r="H81" s="125" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B82" s="79" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C82" s="95">
         <f>MAX(Data!C18,0)</f>
@@ -8235,7 +8242,7 @@
     </row>
     <row r="83" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B83" s="119" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C83" s="100">
         <f>C78-C79-C80-C81-C82/(1-F84)</f>
@@ -8256,7 +8263,7 @@
     </row>
     <row r="84" spans="1:8" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B84" s="28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C84" s="121"/>
       <c r="D84" s="134"/>
@@ -8267,7 +8274,7 @@
     </row>
     <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B85" s="93" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C85" s="118">
         <f>C83*(1-F84)</f>
@@ -8288,7 +8295,7 @@
     </row>
     <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B86" s="94" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C86" s="161">
         <f>C85*Data!E3/Common_Shares</f>
@@ -8303,7 +8310,7 @@
     </row>
     <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B87" s="93" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C87" s="164">
         <v>0.1026</v>
@@ -8327,34 +8334,34 @@
     <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="5"/>
       <c r="B89" s="120" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C89" s="21"/>
       <c r="H89" s="50" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B90" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="D90" s="201" t="s">
-        <v>174</v>
-      </c>
-      <c r="E90" s="201"/>
+        <v>171</v>
+      </c>
+      <c r="D90" s="211" t="s">
+        <v>172</v>
+      </c>
+      <c r="E90" s="211"/>
       <c r="G90" s="94"/>
     </row>
     <row r="91" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B91" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C91" s="174" t="s">
-        <v>225</v>
-      </c>
-      <c r="D91" s="194" t="s">
-        <v>175</v>
-      </c>
-      <c r="E91" s="194"/>
+        <v>222</v>
+      </c>
+      <c r="D91" s="205" t="s">
+        <v>173</v>
+      </c>
+      <c r="E91" s="205"/>
       <c r="F91" s="29">
         <f>E83/C68</f>
         <v>0.10118575838478229</v>
@@ -8370,10 +8377,10 @@
         <f>IF(C91="CN",Dashboard!C17,IF(C91="US",Dashboard!C12,IF(C91="HK",Dashboard!D12,Dashboard!D17)))</f>
         <v>0.08</v>
       </c>
-      <c r="D92" s="194" t="s">
-        <v>171</v>
-      </c>
-      <c r="E92" s="194"/>
+      <c r="D92" s="205" t="s">
+        <v>169</v>
+      </c>
+      <c r="E92" s="205"/>
       <c r="F92" s="137">
         <v>0.02</v>
       </c>
@@ -8392,7 +8399,7 @@
     </row>
     <row r="95" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B95" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C95" s="102">
         <f>E85/(C92-F92)*Exchange_Rate</f>
@@ -8405,7 +8412,7 @@
     </row>
     <row r="96" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B96" s="28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C96" s="102">
         <f>E82*Exchange_Rate</f>
@@ -8420,7 +8427,7 @@
     </row>
     <row r="97" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B97" s="119" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C97" s="123">
         <f>(E65+MIN(0,E70))*Exchange_Rate</f>
@@ -8431,15 +8438,15 @@
         <v>-10.16734853738434</v>
       </c>
       <c r="E97" s="157" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F97" s="158" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B98" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C98" s="102">
         <f>C95-C96+$C$97</f>
@@ -8460,22 +8467,22 @@
     </row>
     <row r="100" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B100" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D100" s="165" t="str">
         <f>D94</f>
         <v>HKD</v>
       </c>
       <c r="E100" s="157" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F100" s="158" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="101" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B101" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C101" s="102">
         <f>D101*Common_Shares/Data!E3</f>
@@ -8496,10 +8503,10 @@
     </row>
     <row r="103" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B103" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C103" s="166" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>